<commit_message>
Correct link to GIFComment
</commit_message>
<xml_diff>
--- a/Documentation/taglist/gif.xlsx
+++ b/Documentation/taglist/gif.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
   <si>
     <t>SHORT</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>GIFComment</t>
+  </si>
+  <si>
+    <t>[GIFComment](xref:ExifLibrary.GIFComment)</t>
   </si>
 </sst>
 </file>
@@ -930,6 +933,17 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
@@ -1108,9 +1122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1214,32 +1226,32 @@
         <v/>
       </c>
       <c r="L2" t="str">
-        <f t="shared" ref="L2:L13" si="0">IF(J2="",H2,H2&amp;" or "&amp;J2)</f>
+        <f t="shared" ref="L2" si="0">IF(J2="",H2,H2&amp;" or "&amp;J2)</f>
         <v>[ExifAscii](xref:ExifLibrary.ExifAscii)</v>
       </c>
       <c r="M2" t="str">
-        <f t="shared" ref="M2:M13" si="1">IF(K2="",I2,I2&amp;" or "&amp;K2)</f>
+        <f t="shared" ref="M2" si="1">IF(K2="",I2,I2&amp;" or "&amp;K2)</f>
         <v>string</v>
       </c>
       <c r="N2" t="b">
         <f>NOT( ISERROR(VLOOKUP($A2,'Custom Types'!$A$2:$A$997,1,FALSE)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2" t="str">
-        <f t="shared" ref="O2:O13" si="2">"["&amp;A2&amp;"](xref:ExifLibrary.ExifTag."&amp;A2&amp;")"</f>
+        <f t="shared" ref="O2" si="2">"["&amp;A2&amp;"](xref:ExifLibrary.ExifTag."&amp;A2&amp;")"</f>
         <v>[GIFComment](xref:ExifLibrary.ExifTag.GIFComment)</v>
       </c>
       <c r="P2" t="str">
         <f>IF($N2,VLOOKUP($A2,'Custom Types'!$A$2:$C$997,2,FALSE),L2)</f>
-        <v>[ExifAscii](xref:ExifLibrary.ExifAscii)</v>
+        <v>[GIFComment](xref:ExifLibrary.GIFComment)</v>
       </c>
       <c r="Q2" t="str">
         <f>IF($N2,VLOOKUP($A2,'Custom Types'!$A$2:$C$997,3,FALSE),M2)</f>
         <v>string</v>
       </c>
       <c r="R2" t="str">
-        <f t="shared" ref="R2:R13" si="3">O2&amp;" | "&amp;B2&amp;" | "&amp;C2&amp;" | "&amp;P2&amp;" | "&amp;Q2</f>
-        <v>[GIFComment](xref:ExifLibrary.ExifTag.GIFComment) | 0 | 0x0000 | [ExifAscii](xref:ExifLibrary.ExifAscii) | string</v>
+        <f t="shared" ref="R2" si="3">O2&amp;" | "&amp;B2&amp;" | "&amp;C2&amp;" | "&amp;P2&amp;" | "&amp;Q2</f>
+        <v>[GIFComment](xref:ExifLibrary.ExifTag.GIFComment) | 0 | 0x0000 | [GIFComment](xref:ExifLibrary.GIFComment) | string</v>
       </c>
     </row>
   </sheetData>

</xml_diff>